<commit_message>
Update time tracking for sprint 5
</commit_message>
<xml_diff>
--- a/Time Tracking/Project Time Tracking Dustin_Shaver.xlsx
+++ b/Time Tracking/Project Time Tracking Dustin_Shaver.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dustin\Documents\School\SW Dev Tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dustin\Documents\School\SW Dev Tools\Time Tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B80357DD-A7A4-4CDD-A1D9-EC5E64D4B951}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE453FFB-F9CA-444C-867B-BDFF60DC51D5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{E7129392-AEC3-481D-9E4A-CBA8FF9BF1AA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="47">
   <si>
     <t>Time Tracking</t>
   </si>
@@ -154,6 +154,18 @@
   </si>
   <si>
     <t>Tested Canvas resize bug fix. Dirty resize does not work. Will make canvas static size.</t>
+  </si>
+  <si>
+    <t>Designing architecture to store layer data and use that data to update the image export file.</t>
+  </si>
+  <si>
+    <t>Fix bugs associated with larger brush event handlers. Integrated brush handlers to edit image data.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final testing and debug of sprint integration, including event handlers for canvas resize and new canvas methods. </t>
+  </si>
+  <si>
+    <t>Project Total</t>
   </si>
 </sst>
 </file>
@@ -205,13 +217,13 @@
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -530,7 +542,7 @@
   <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -540,22 +552,22 @@
     <col min="3" max="3" width="14.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" style="1" customWidth="1"/>
     <col min="5" max="6" width="20.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="41.28515625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="41.28515625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
     </row>
     <row r="2" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -576,16 +588,16 @@
       <c r="F2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
     </row>
     <row r="3" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -607,7 +619,7 @@
       <c r="F3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="6" t="s">
         <v>8</v>
       </c>
       <c r="H3" t="s">
@@ -638,7 +650,7 @@
       <c r="F4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="6" t="s">
         <v>9</v>
       </c>
       <c r="H4" s="5" t="s">
@@ -669,7 +681,7 @@
       <c r="F5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H5" t="s">
@@ -700,7 +712,7 @@
       <c r="F6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="6" t="s">
         <v>11</v>
       </c>
       <c r="H6" t="s">
@@ -731,11 +743,15 @@
       <c r="F7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H7" t="s">
         <v>24</v>
+      </c>
+      <c r="I7" s="5">
+        <f>SUM(D24:D26)</f>
+        <v>0.35347222222222224</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -758,7 +774,7 @@
       <c r="F8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="6" t="s">
         <v>14</v>
       </c>
       <c r="H8" t="s">
@@ -785,9 +801,13 @@
       <c r="F9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="6" t="s">
         <v>27</v>
       </c>
+      <c r="H9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I9" s="5"/>
     </row>
     <row r="10" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -809,7 +829,7 @@
       <c r="F10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="6" t="s">
         <v>16</v>
       </c>
     </row>
@@ -833,7 +853,7 @@
       <c r="F11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="6" t="s">
         <v>28</v>
       </c>
     </row>
@@ -857,7 +877,7 @@
       <c r="F12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -881,7 +901,7 @@
       <c r="F13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="6" t="s">
         <v>29</v>
       </c>
     </row>
@@ -905,7 +925,7 @@
       <c r="F14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G14" s="6" t="s">
         <v>31</v>
       </c>
     </row>
@@ -929,7 +949,7 @@
       <c r="F15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="G15" s="6" t="s">
         <v>33</v>
       </c>
     </row>
@@ -953,7 +973,7 @@
       <c r="F16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="G16" s="6" t="s">
         <v>34</v>
       </c>
     </row>
@@ -977,7 +997,7 @@
       <c r="F17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="G17" s="6" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1001,7 +1021,7 @@
       <c r="F18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="G18" s="6" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1025,7 +1045,7 @@
       <c r="F19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G19" s="7" t="s">
+      <c r="G19" s="6" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1049,7 +1069,7 @@
       <c r="F20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="G20" s="6" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1073,7 +1093,7 @@
       <c r="F21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G21" s="7" t="s">
+      <c r="G21" s="6" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1097,7 +1117,7 @@
       <c r="F22" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G22" s="7" t="s">
+      <c r="G22" s="6" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1121,26 +1141,80 @@
       <c r="F23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G23" s="7" t="s">
+      <c r="G23" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>43571</v>
+      </c>
+      <c r="B24" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0.54166666666666663</v>
+      </c>
       <c r="D24" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.12499999999999994</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>43573</v>
+      </c>
+      <c r="B25" s="3">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0.64722222222222225</v>
+      </c>
       <c r="D25" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.13680555555555562</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>43579</v>
+      </c>
+      <c r="B26" s="3">
+        <v>0.59027777777777779</v>
+      </c>
+      <c r="C26" s="3">
+        <v>0.68194444444444446</v>
+      </c>
       <c r="D26" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9.1666666666666674E-2</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update time tracking Dustin Shaver
</commit_message>
<xml_diff>
--- a/Time Tracking/Project Time Tracking Dustin_Shaver.xlsx
+++ b/Time Tracking/Project Time Tracking Dustin_Shaver.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dustin\Documents\School\SW Dev Tools\Time Tracking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dustin\Documents\School\SW Dev Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE453FFB-F9CA-444C-867B-BDFF60DC51D5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E34863-26AD-4298-B0D5-3EB06CE24559}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{E7129392-AEC3-481D-9E4A-CBA8FF9BF1AA}"/>
   </bookViews>
@@ -20,12 +20,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="52">
   <si>
     <t>Time Tracking</t>
   </si>
@@ -166,6 +171,21 @@
   </si>
   <si>
     <t>Project Total</t>
+  </si>
+  <si>
+    <t>Testing/Organization</t>
+  </si>
+  <si>
+    <t>Prototyed, implemented, and tested final canvas method. Fixed resize but in canvas class. Merged event handlers for menu/color panel.</t>
+  </si>
+  <si>
+    <t>Designed and implemented the layer system patch in the layer panel class to allow the proper creation and connection of the layers to the canvas.</t>
+  </si>
+  <si>
+    <t>Tested final canvas objects. Fixed bug in the new canvas button/class. Worked on implementing layer panel. Attempted, but failed to impliment layer merging.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Updated canvas comments and code. Removed testing lines and redundent code. Formatted for improved readability. </t>
   </si>
 </sst>
 </file>
@@ -201,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -221,6 +241,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -541,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{543D8B75-6D61-468C-A840-B72F142D43E2}">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:XFD31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -557,17 +580,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
     </row>
     <row r="2" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -591,13 +614,13 @@
       <c r="G2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
     </row>
     <row r="3" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -1217,28 +1240,100 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>43584</v>
+      </c>
+      <c r="B27" s="3">
+        <v>0.59027777777777779</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0.77777777777777779</v>
+      </c>
       <c r="D27" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.1875</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>43587</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0.58680555555555558</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0.69097222222222221</v>
+      </c>
       <c r="D28" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.10416666666666663</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>43588</v>
+      </c>
+      <c r="B29" s="3">
+        <v>0.64097222222222217</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0.75</v>
+      </c>
       <c r="D29" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.10902777777777783</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>43589</v>
+      </c>
+      <c r="B30" s="3">
+        <v>0.60763888888888895</v>
+      </c>
+      <c r="C30" s="3">
+        <v>0.78819444444444453</v>
+      </c>
       <c r="D30" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.18055555555555558</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1246,12 +1341,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F31" s="8"/>
     </row>
     <row r="32" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D32" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F32" s="8"/>
     </row>
     <row r="33" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D33" s="3">

</xml_diff>